<commit_message>
more buttons and smoothing
</commit_message>
<xml_diff>
--- a/AbletonControls.xlsx
+++ b/AbletonControls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\whous\OneDrive\Desktop\Software Projects\Side Projects\Playstation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A637977-6E57-4203-B66C-24A391434031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40979B9-E653-4770-B44E-EFD2E2C348B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,7 +574,7 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="A14" sqref="A14:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,76 +728,76 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" s="2">
-        <v>0</v>
-      </c>
-      <c r="C18" t="s">
-        <v>46</v>
-      </c>
+      <c r="A18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B19" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -805,32 +805,32 @@
         <v>57</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>58</v>
       </c>
-      <c r="B22" t="s">
-        <v>41</v>
+      <c r="B22" s="2">
+        <v>0</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="C23" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
feeling like it might be done for now
</commit_message>
<xml_diff>
--- a/AbletonControls.xlsx
+++ b/AbletonControls.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\whous\OneDrive\Desktop\Software Projects\Side Projects\Playstation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40979B9-E653-4770-B44E-EFD2E2C348B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D2AD9D-F4EC-4DCA-B5D0-3336B1CE06BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="66">
   <si>
     <t>Control</t>
   </si>
@@ -135,12 +135,6 @@
     <t>L2 + X</t>
   </si>
   <si>
-    <t>Ctrl (hold)</t>
-  </si>
-  <si>
-    <t>Shift (hold)</t>
-  </si>
-  <si>
     <t>R1</t>
   </si>
   <si>
@@ -180,9 +174,6 @@
     <t>The below are not coded yet</t>
   </si>
   <si>
-    <t>Ctrl</t>
-  </si>
-  <si>
     <t>R2 + Square</t>
   </si>
   <si>
@@ -231,17 +222,14 @@
     <t>Enter</t>
   </si>
   <si>
-    <t xml:space="preserve">Shift </t>
-  </si>
-  <si>
-    <t>R2 + L1</t>
+    <t>Shift</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,7 +240,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF61FF87"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF61FF87"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -267,12 +262,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -280,23 +275,87 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF61FF87"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -571,325 +630,340 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD17"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B13" t="s">
-        <v>67</v>
-      </c>
-      <c r="C13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="6">
+        <v>0</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>53</v>
-      </c>
-      <c r="B15" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>54</v>
-      </c>
-      <c r="B16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B20" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>58</v>
-      </c>
-      <c r="B22" s="2">
-        <v>0</v>
-      </c>
-      <c r="C22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>69</v>
-      </c>
-      <c r="B23" t="s">
-        <v>68</v>
-      </c>
-      <c r="C23" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B31" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B24" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B32" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B25" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B26" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="B34" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B27" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>2</v>
-      </c>
-      <c r="B28" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>65</v>
-      </c>
-      <c r="B29" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>66</v>
-      </c>
-      <c r="B30" t="s">
-        <v>64</v>
+      <c r="B35" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>